<commit_message>
adding testing method for auto evaluating
</commit_message>
<xml_diff>
--- a/CVS Files/01.08.22/annotation/GOLD vs Clusters.xlsx
+++ b/CVS Files/01.08.22/annotation/GOLD vs Clusters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USERS-Load\PycharmProjects\pythonProject\CVS Files\01.08.22\annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB58A420-F75F-4937-A9FD-042B8CA0F648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57424F1C-C2FB-48F8-B174-63BD5434C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding the implemention of the auto evaluating
</commit_message>
<xml_diff>
--- a/CVS Files/01.08.22/annotation/GOLD vs Clusters.xlsx
+++ b/CVS Files/01.08.22/annotation/GOLD vs Clusters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USERS-Load\PycharmProjects\pythonProject\CVS Files\01.08.22\annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57424F1C-C2FB-48F8-B174-63BD5434C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0478E6A7-D0E7-4C4A-A22F-E6E7AE2FF03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="143">
   <si>
     <t>text</t>
   </si>
@@ -402,6 +402,60 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>The accuracy is  87.04686118479222</t>
+  </si>
+  <si>
+    <t>The percision is  26.02965403624382</t>
+  </si>
+  <si>
+    <t>The recall is  26.87074829931973</t>
+  </si>
+  <si>
+    <t>purity =  49.572649572649574</t>
+  </si>
+  <si>
+    <t>the count of tp is 158</t>
+  </si>
+  <si>
+    <t>the count of tn is 5749</t>
+  </si>
+  <si>
+    <t>the count of fn is 430</t>
+  </si>
+  <si>
+    <t>the count of fb is 449</t>
+  </si>
+  <si>
+    <t>Auto calculated using cosin similarity for 10 essays</t>
+  </si>
+  <si>
+    <t>the value of tp is 86</t>
+  </si>
+  <si>
+    <t>the value of tn is 2955</t>
+  </si>
+  <si>
+    <t>the value of fn is 74</t>
+  </si>
+  <si>
+    <t>the value of fb is 206</t>
+  </si>
+  <si>
+    <t>The accuracy is  91.56880457693465</t>
+  </si>
+  <si>
+    <t>The percision is  29.45205479452055</t>
+  </si>
+  <si>
+    <t>The recall is  53.75</t>
+  </si>
+  <si>
+    <t>purity =  70.73170731707317</t>
+  </si>
+  <si>
+    <t>Auto calculated using cosin similarity for 5 items of each cluster</t>
   </si>
 </sst>
 </file>
@@ -424,7 +478,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,6 +539,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -498,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -514,6 +580,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,16 +864,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="112.77734375" customWidth="1"/>
+    <col min="2" max="2" width="141.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="7" max="7" width="60.21875" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
@@ -2419,6 +2488,10 @@
       <c r="D25" s="4">
         <v>16</v>
       </c>
+      <c r="G25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -2433,6 +2506,10 @@
       <c r="D26" s="4">
         <v>16</v>
       </c>
+      <c r="G26" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -2447,6 +2524,10 @@
       <c r="D27" s="4">
         <v>16</v>
       </c>
+      <c r="G27" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -2461,6 +2542,10 @@
       <c r="D28" s="4">
         <v>13</v>
       </c>
+      <c r="G28" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -2475,6 +2560,10 @@
       <c r="D29" s="4">
         <v>13</v>
       </c>
+      <c r="G29" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -2489,6 +2578,10 @@
       <c r="D30" s="4">
         <v>13</v>
       </c>
+      <c r="G30" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -2503,6 +2596,10 @@
       <c r="D31" s="4">
         <v>16</v>
       </c>
+      <c r="G31" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -2517,8 +2614,12 @@
       <c r="D32" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G32" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2532,7 +2633,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2545,8 +2646,12 @@
       <c r="D34" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G34" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2560,7 +2665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2574,7 +2679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2588,7 +2693,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2601,8 +2706,11 @@
       <c r="D38" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G38" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2615,8 +2723,11 @@
       <c r="D39" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G39" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2629,8 +2740,11 @@
       <c r="D40" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G40" s="13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2643,8 +2757,11 @@
       <c r="D41" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G41" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2657,8 +2774,11 @@
       <c r="D42" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G42" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2671,8 +2791,11 @@
       <c r="D43" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G43" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2685,8 +2808,11 @@
       <c r="D44" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G44" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2699,8 +2825,11 @@
       <c r="D45" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G45" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2713,8 +2842,11 @@
       <c r="D46" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G46" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2728,7 +2860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>

</xml_diff>